<commit_message>
Add License column (#563)
</commit_message>
<xml_diff>
--- a/static/download_template/wells.xlsx
+++ b/static/download_template/wells.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">License</t>
   </si>
   <si>
     <t xml:space="preserve">As recorded in the original database.</t>
@@ -172,6 +175,12 @@
     <t xml:space="preserve">The address of the data point.</t>
   </si>
   <si>
+    <t xml:space="preserve">License type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restriction</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aquifer Name</t>
   </si>
   <si>
@@ -224,9 +233,6 @@
   </si>
   <si>
     <t xml:space="preserve">Number of people served </t>
-  </si>
-  <si>
-    <t xml:space="preserve">License</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -401,12 +407,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -472,23 +478,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF77933C"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16:C30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R14" activeCellId="0" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="16" style="2" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="15.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="17" style="2" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -530,61 +536,71 @@
       <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="0"/>
+      <c r="O1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="3"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="M2" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -593,7 +609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF77933C"/>
     <pageSetUpPr fitToPage="false"/>
@@ -601,14 +617,13 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="1" sqref="C16:C30 Q1"/>
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="9" style="2" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1019" min="9" style="2" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -616,54 +631,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="P1" s="4"/>
       <c r="Q1" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -673,7 +688,7 @@
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -684,23 +699,23 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O2" s="6"/>
       <c r="P2" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="S2" s="6"/>
     </row>
@@ -713,8 +728,8 @@
     <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -723,7 +738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF77933C"/>
     <pageSetUpPr fitToPage="false"/>
@@ -731,14 +746,13 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C16:C30 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1010" min="11" style="2" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1011" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1010" min="11" style="2" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -746,27 +760,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="ALW1" s="0"/>
       <c r="ALX1" s="0"/>
@@ -785,13 +799,13 @@
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
@@ -799,13 +813,13 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>5</v>
@@ -817,8 +831,8 @@
     <mergeCell ref="G1:J1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Add glo_90m to ods
</commit_message>
<xml_diff>
--- a/static/download_template/wells.xlsx
+++ b/static/download_template/wells.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -55,6 +55,9 @@
   <si>
     <t xml:space="preserve">Ground surface elevation
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEM elevation based on the GLO_90m dataset </t>
   </si>
   <si>
     <t xml:space="preserve">Top of well elevation</t>
@@ -279,6 +282,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Unit must be either:
 </t>
@@ -289,6 +293,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -299,6 +304,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Domestic
 </t>
@@ -309,6 +315,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -319,6 +326,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Irrigation
 </t>
@@ -329,6 +337,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -339,6 +348,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Livestock
 </t>
@@ -349,6 +359,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -359,6 +370,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Industrial
 </t>
@@ -369,6 +381,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -379,6 +392,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Services (e.g. tourism)</t>
     </r>
@@ -402,7 +416,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -447,19 +461,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -530,7 +531,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -560,10 +561,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,18 +642,18 @@
     <tabColor rgb="FF77933C"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="15.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="17" style="2" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="15.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="19" style="2" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -692,73 +689,83 @@
         <v>9</v>
       </c>
       <c r="L1" s="4"/>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="AMJ1" s="0"/>
+      <c r="Q1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="N2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>27</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -779,7 +786,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="K2:L2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -793,54 +800,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P1" s="4"/>
       <c r="Q1" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -850,38 +857,38 @@
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O2" s="6"/>
       <c r="P2" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S2" s="6"/>
     </row>
@@ -912,7 +919,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="K2:L2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -926,27 +933,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="ALW1" s="0"/>
       <c r="ALX1" s="0"/>
@@ -965,29 +972,29 @@
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>53</v>
+      <c r="E2" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add glo_90m_elevation field (#136)
* Add glo_90m_elevation field

* Add glo_90m to ods
</commit_message>
<xml_diff>
--- a/static/download_template/wells.xlsx
+++ b/static/download_template/wells.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -55,6 +55,9 @@
   <si>
     <t xml:space="preserve">Ground surface elevation
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEM elevation based on the GLO_90m dataset </t>
   </si>
   <si>
     <t xml:space="preserve">Top of well elevation</t>
@@ -279,6 +282,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Unit must be either:
 </t>
@@ -289,6 +293,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -299,6 +304,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Domestic
 </t>
@@ -309,6 +315,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -319,6 +326,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Irrigation
 </t>
@@ -329,6 +337,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -339,6 +348,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Livestock
 </t>
@@ -349,6 +359,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -359,6 +370,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Industrial
 </t>
@@ -369,6 +381,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">•</t>
     </r>
@@ -379,6 +392,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Services (e.g. tourism)</t>
     </r>
@@ -402,7 +416,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -447,19 +461,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -530,7 +531,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -560,10 +561,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,18 +642,18 @@
     <tabColor rgb="FF77933C"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="15.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="17" style="2" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="15.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="19" style="2" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -692,73 +689,83 @@
         <v>9</v>
       </c>
       <c r="L1" s="4"/>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="AMJ1" s="0"/>
+      <c r="Q1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="N2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>27</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -779,7 +786,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="K2:L2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -793,54 +800,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P1" s="4"/>
       <c r="Q1" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -850,38 +857,38 @@
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O2" s="6"/>
       <c r="P2" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S2" s="6"/>
     </row>
@@ -912,7 +919,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="K2:L2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -926,27 +933,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="ALW1" s="0"/>
       <c r="ALX1" s="0"/>
@@ -965,29 +972,29 @@
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>53</v>
+      <c r="E2" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add first and last measurements
</commit_message>
<xml_diff>
--- a/static/download_template/wells.xlsx
+++ b/static/download_template/wells.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t xml:space="preserve">License</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measurement Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measurement Data</t>
   </si>
   <si>
     <t xml:space="preserve">As recorded in the original database.</t>
@@ -182,6 +188,29 @@
   </si>
   <si>
     <t xml:space="preserve">Restriction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groundwater levels:
+• Yes
+• No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groundwater quality:
+• Yes
+• No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abstraction / Discharge:
+• Yes
+• No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Measurement  
+(READ ONLY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Measurement  
+(READ ONLY)</t>
   </si>
   <si>
     <t xml:space="preserve">Aquifer Name</t>
@@ -416,7 +445,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -455,11 +484,27 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -531,7 +576,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -552,11 +597,19 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -642,10 +695,10 @@
     <tabColor rgb="FF77933C"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:L2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S15" activeCellId="0" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -656,7 +709,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="19" style="2" width="15.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -703,69 +756,95 @@
         <v>13</v>
       </c>
       <c r="R1" s="3"/>
+      <c r="S1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="K2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="N2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="P2" s="7" t="s">
         <v>28</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -786,7 +865,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="K2:L2 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -795,59 +874,59 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1019" min="9" style="2" width="15.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="P1" s="4"/>
       <c r="Q1" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -856,41 +935,41 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="6"/>
+      <c r="A2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="N2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="7"/>
+      <c r="P2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -919,7 +998,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="K2:L2 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -928,20 +1007,20 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1010" min="11" style="2" width="15.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>13</v>
@@ -950,10 +1029,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="ALW1" s="0"/>
       <c r="ALX1" s="0"/>
@@ -971,32 +1050,32 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="A2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="E2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add measurement type on model
</commit_message>
<xml_diff>
--- a/static/download_template/wells.xlsx
+++ b/static/download_template/wells.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -196,11 +196,6 @@
   </si>
   <si>
     <t xml:space="preserve">Groundwater quality:
-• Yes
-• No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abstraction / Discharge:
 • Yes
 • No</t>
   </si>
@@ -695,10 +690,10 @@
     <tabColor rgb="FF77933C"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S15" activeCellId="0" sqref="S15"/>
+      <selection pane="topLeft" activeCell="V13" activeCellId="0" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -706,7 +701,8 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="15.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="15.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="19" style="2" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="19" style="2" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -760,11 +756,11 @@
         <v>14</v>
       </c>
       <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -832,9 +828,6 @@
       </c>
       <c r="V2" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -843,8 +836,8 @@
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -879,54 +872,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P1" s="4"/>
       <c r="Q1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -936,38 +929,38 @@
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O2" s="7"/>
       <c r="P2" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q2" s="7"/>
       <c r="R2" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S2" s="7"/>
     </row>
@@ -1012,15 +1005,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>13</v>
@@ -1029,10 +1022,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="ALW1" s="0"/>
       <c r="ALX1" s="0"/>
@@ -1051,29 +1044,29 @@
     </row>
     <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
File updates for download
</commit_message>
<xml_diff>
--- a/static/download_template/wells.xlsx
+++ b/static/download_template/wells.xlsx
@@ -5,34 +5,32 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Hydrogeology" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Management" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'general information '!#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'general information '!#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'general information '!#ref!</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Name </t>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data provider</t>
   </si>
   <si>
     <t xml:space="preserve">Feature Type</t>
@@ -63,6 +61,9 @@
     <t xml:space="preserve">Top of well elevation</t>
   </si>
   <si>
+    <t xml:space="preserve">Data quality flag</t>
+  </si>
+  <si>
     <t xml:space="preserve">Country</t>
   </si>
   <si>
@@ -84,11 +85,13 @@
     <t xml:space="preserve">The name of the data point.</t>
   </si>
   <si>
+    <t xml:space="preserve">GGIS organisation name</t>
+  </si>
+  <si>
     <t xml:space="preserve">One of the following:
-• Borehole
-• Hand-dug well
+• Water well
 • Spring
-If the feature type list does not include the type you need, contact the GGIS administrator : ggis@un-igrac.org.</t>
+• Other</t>
   </si>
   <si>
     <t xml:space="preserve">One of the following:
@@ -118,76 +121,30 @@
     <t xml:space="preserve">Measured Above Mean Sea Level (AMSL).</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Unit must be either:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">•</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> m
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">•</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> ft</t>
-    </r>
+    <t xml:space="preserve">Unit must be either:
+• m
+• ft</t>
   </si>
   <si>
     <t xml:space="preserve">Measured Above Mean Sea Level (AMSL). The top of the well is usually higher than the ground surface elevation.</t>
   </si>
   <si>
+    <t xml:space="preserve">Is there a gap of more than 3 years in the groundwater level time series?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there a jump of +50 or -50 m in the groundwater level time series?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there a suspicious groundwater level value? (e.g. 9999, exactly zero)</t>
+  </si>
+  <si>
     <t xml:space="preserve">3-letters ISO code of the country. See for example: https://en.wikipedia.org/wiki/ISO_3166-1_alpha-3#Officially_assigned_code_elements</t>
   </si>
   <si>
     <t xml:space="preserve">The address of the data point.</t>
   </si>
   <si>
-    <t xml:space="preserve">License type.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restriction.</t>
+    <t xml:space="preserve">Licence under which the data is shared by the provider</t>
   </si>
   <si>
     <t xml:space="preserve">Groundwater levels:
@@ -200,11 +157,11 @@
 • No</t>
   </si>
   <si>
-    <t xml:space="preserve">First Measurement  
+    <t xml:space="preserve">First Measurement
 (READ ONLY)</t>
   </si>
   <si>
-    <t xml:space="preserve">Last Measurement  
+    <t xml:space="preserve">Last Measurement
 (READ ONLY)</t>
   </si>
   <si>
@@ -284,153 +241,18 @@
 • m³/s</t>
   </si>
   <si>
-    <t xml:space="preserve">Organisation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Groundwater use</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of people served </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manager / owner</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Unit must be either:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">•</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Domestic
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">•</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Irrigation
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">•</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Livestock
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">•</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Industrial
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">•</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Services (e.g. tourism)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valid from 
-(yyyy-mm-dd )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valid until 
-(yyyy-mm-dd)</t>
+    <t xml:space="preserve">Number of people served</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit must be either:
+• Domestic
+• Irrigation
+• Livestock
+• Industrial
+• Services (e.g. tourism)</t>
   </si>
 </sst>
 </file>
@@ -440,13 +262,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -467,16 +288,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -484,15 +296,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -500,7 +303,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -535,14 +337,14 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -580,11 +382,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -592,20 +398,16 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -690,161 +492,177 @@
     <tabColor rgb="FF77933C"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="15.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="19" style="2" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="1" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="22" style="3" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="3" width="6.85"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="3" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="O1" s="5"/>
+      <c r="P1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="5"/>
       <c r="U1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="5"/>
-      <c r="AMJ1" s="0"/>
+      <c r="V1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" s="5"/>
     </row>
-    <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="159.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>34</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.75" footer="0.75"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="true" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -858,114 +676,110 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="10" style="2" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="1" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="10" style="3" width="12.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1021" style="2" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="2" width="6.85"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="5"/>
+      <c r="T1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AMG1" s="8"/>
+      <c r="AMH1" s="8"/>
+      <c r="AMI1" s="8"/>
+      <c r="AMJ1" s="8"/>
     </row>
-    <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="159.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="9" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R2" s="7"/>
       <c r="S2" s="9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="T2" s="7"/>
     </row>
@@ -978,11 +792,13 @@
     <mergeCell ref="R1:S1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.75" footer="0.75"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="true" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -995,104 +811,73 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1011" min="12" style="2" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1004" min="5" style="3" width="12.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1017" min="1005" style="2" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="2" width="6.85"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="ALX1" s="0"/>
-      <c r="ALY1" s="0"/>
-      <c r="ALZ1" s="0"/>
-      <c r="AMA1" s="0"/>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="C1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="ALQ1" s="8"/>
+      <c r="ALR1" s="8"/>
+      <c r="ALS1" s="8"/>
+      <c r="ALT1" s="8"/>
+      <c r="ALU1" s="8"/>
+      <c r="ALV1" s="8"/>
+      <c r="ALW1" s="8"/>
+      <c r="ALX1" s="8"/>
+      <c r="ALY1" s="8"/>
+      <c r="ALZ1" s="8"/>
+      <c r="AMA1" s="8"/>
+      <c r="AMB1" s="8"/>
+      <c r="AMC1" s="8"/>
+      <c r="AMD1" s="2"/>
+      <c r="AME1" s="2"/>
+      <c r="AMF1" s="2"/>
+      <c r="AMG1" s="2"/>
+      <c r="AMH1" s="2"/>
+      <c r="AMI1" s="2"/>
+      <c r="AMJ1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="159.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="D2" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="H1:K1"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.75" footer="0.75"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="true" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>